<commit_message>
updated test output files
</commit_message>
<xml_diff>
--- a/indigo_app/tests/xlsx_exporter/commencements_passive_later_output_expected.xlsx
+++ b/indigo_app/tests/xlsx_exporter/commencements_passive_later_output_expected.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robley/code/work/indigo/indigo_app/tests/xlsx_exporter/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB72FA4-62BE-2D47-AF88-BCEFCE0C3D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25640" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Works" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>country</t>
   </si>
@@ -173,9 +179,6 @@
   </si>
   <si>
     <t>/akn/za/act/2020/4 - Commenced_by only</t>
-  </si>
-  <si>
-    <t>(unknown)</t>
   </si>
   <si>
     <t>Commencement notice 1</t>
@@ -211,14 +214,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,15 +254,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -299,7 +318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,9 +350,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,6 +402,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,14 +595,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="21.33203125" customWidth="1"/>
+    <col min="23" max="23" width="22.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +706,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -680,7 +741,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -715,7 +776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -744,7 +805,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -763,8 +824,8 @@
       <c r="O5" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>53</v>
+      <c r="P5" s="2">
+        <v>2958101</v>
       </c>
       <c r="AB5" t="s">
         <v>36</v>
@@ -776,15 +837,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
         <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -808,21 +869,21 @@
         <v>36</v>
       </c>
       <c r="AC6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
         <v>54</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
@@ -839,28 +900,28 @@
       <c r="V7" t="s">
         <v>52</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>53</v>
+      <c r="W7" s="2">
+        <v>2958101</v>
       </c>
       <c r="AB7" t="s">
         <v>36</v>
       </c>
       <c r="AC7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
       <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
         <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>58</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -872,21 +933,21 @@
         <v>36</v>
       </c>
       <c r="AC8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8" t="s">
         <v>59</v>
       </c>
-      <c r="AD8" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
         <v>61</v>
-      </c>
-      <c r="E9" t="s">
-        <v>62</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -910,7 +971,7 @@
         <v>36</v>
       </c>
       <c r="AC9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD9" t="s">
         <v>39</v>

</xml_diff>